<commit_message>
Remarks : file updated with tc no - 16,17
</commit_message>
<xml_diff>
--- a/TCS_NEWUI_Multiple Product Frontend functionality.xlsx
+++ b/TCS_NEWUI_Multiple Product Frontend functionality.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sumit Rana\Projects\AdIntel- New\Test Cases\Completed\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2292AF19-3506-4366-A307-73AE2F9E3E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" tabRatio="815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="5" r:id="rId1"/>
@@ -41,7 +35,7 @@
     <definedName name="test" localSheetId="2">#REF!</definedName>
     <definedName name="test">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -54,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="167">
   <si>
     <t>Test Case Result Modules-Wise</t>
   </si>
@@ -518,10 +512,6 @@
   </si>
   <si>
     <t>Export the AgGrid Report in Creative AssetsFormat by clicking the Export FAB button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.The Exported file should show multiple files of creative respective of no. of multiproduct (For eg if one AdcODE contains 3 multi product then it will show 3 creative assests downloaded file)
-2.The Exported File should not show Multiple entries of Records of the AdCode product </t>
   </si>
   <si>
     <t>Verify Creative Asset export for Multiple Product for selected record</t>
@@ -602,11 +592,21 @@
   <si>
     <t>Only one primary product should be displayed in schedule alerts emails</t>
   </si>
+  <si>
+    <t>SMRT-7853</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Only one file should Exported for one product/Ad (It should not download multiple file)
+</t>
+  </si>
+  <si>
+    <t>US:WEB-7573_TC 17</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -2097,7 +2097,7 @@
     <xf numFmtId="41" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="92" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="134"/>
@@ -2260,15 +2260,6 @@
     <xf numFmtId="0" fontId="45" fillId="31" borderId="33" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="31" borderId="33" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="31" borderId="33" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="31" borderId="33" xfId="144" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="46" fillId="31" borderId="33" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2286,6 +2277,9 @@
     <xf numFmtId="0" fontId="50" fillId="31" borderId="33" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="33" xfId="144" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="26" borderId="7" xfId="134" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2316,6 +2310,24 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="30" borderId="39" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="30" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="30" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="39" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="28" borderId="39" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2325,24 +2337,6 @@
     <xf numFmtId="0" fontId="6" fillId="28" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="39" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="30" borderId="39" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="30" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="30" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="34" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2363,163 +2357,163 @@
     </xf>
   </cellXfs>
   <cellStyles count="157">
-    <cellStyle name="20% - Accent1" xfId="11" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent1 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 2 3" xfId="13" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 2 3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent1 2 2 2 2 3 3" xfId="20" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - Accent1 2 3" xfId="22" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="20% - Accent1 2 3 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - Accent1 2 3 2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="20% - Accent1 2 3 2 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - Accent1 2 3 2 4" xfId="29" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="20% - Accent2" xfId="30" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="20% - Accent2 2 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 2 3" xfId="34" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 2 3 2" xfId="36" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="20% - Accent2 2 2 2 2 3 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="20% - Accent2 2 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="20% - Accent2 2 3 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="20% - Accent3" xfId="39" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="20% - Accent4" xfId="40" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="20% - Accent5" xfId="42" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="20% - Accent6" xfId="16" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="40% - Accent1" xfId="3" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="40% - Accent1 2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="40% - Accent1 2 2 2 2 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="40% - Accent1 2 2 2 2 3 2 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="40% - Accent1 2 2 2 2 3 2 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="40% - Accent1 2 3" xfId="54" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="40% - Accent1 2 3 2" xfId="55" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="40% - Accent2" xfId="12" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="40% - Accent2 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="40% - Accent2 2 2 2 2 3 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="40% - Accent2 2 2 2 2 3 2 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="40% - Accent2 2 2 2 2 3 2 3" xfId="31" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="40% - Accent2 2 3" xfId="58" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="40% - Accent2 2 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="40% - Accent2 2 3 2 2" xfId="138" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="40% - Accent2 2 3 2 2 2" xfId="150" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="40% - Accent3" xfId="6" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="40% - Accent4" xfId="21" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="40% - Accent5" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="40% - Accent6" xfId="53" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="60% - Accent1" xfId="41" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="60% - Accent2" xfId="14" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="60% - Accent3" xfId="18" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="60% - Accent4" xfId="47" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="60% - Accent5" xfId="63" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="60% - Accent6" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Accent1" xfId="64" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Accent1 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Accent1 2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Accent1 2 2 2 2 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Accent1 2 2 2 2 3 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Accent1 2 2 2 2 3 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Accent1 2 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Accent1 2 3 2" xfId="69" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Accent1 2 3 2 2" xfId="135" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Accent2" xfId="70" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Accent2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Accent2 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Accent2 2 2 2 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Accent2 2 2 2 2 3 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Accent2 2 2 2 2 3 3" xfId="73" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Accent2 2 3" xfId="74" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Accent2 2 3 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Accent2 2 3 2 2" xfId="136" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Accent3" xfId="76" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Accent4" xfId="23" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Accent5" xfId="77" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Accent6" xfId="26" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Bad" xfId="78" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Calculation" xfId="8" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Check Cell" xfId="79" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Comma [0] 2" xfId="155" xr:uid="{4E8A59C3-F7FB-4433-84F9-1A1256A1DBD1}"/>
-    <cellStyle name="Comma [0] 3" xfId="156" xr:uid="{44AC3AAC-7079-4FD8-B5F5-B58B0B18BA35}"/>
-    <cellStyle name="Explanatory Text" xfId="80" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Good" xfId="81" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Heading 1" xfId="82" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Heading 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Heading 2 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Heading 2 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Heading 2 2 2 2 2 3 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Heading 2 2 2 2 2 3 2 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Heading 2 2 2 2 2 3 2 3" xfId="89" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Heading 2 2 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Heading 2 2 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Heading 3" xfId="90" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Heading 4" xfId="91" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="20% - Accent1" xfId="11"/>
+    <cellStyle name="20% - Accent1 2" xfId="2"/>
+    <cellStyle name="20% - Accent1 2 2" xfId="7"/>
+    <cellStyle name="20% - Accent1 2 2 2 2 3" xfId="13"/>
+    <cellStyle name="20% - Accent1 2 2 2 2 3 2" xfId="17"/>
+    <cellStyle name="20% - Accent1 2 2 2 2 3 3" xfId="20"/>
+    <cellStyle name="20% - Accent1 2 3" xfId="22"/>
+    <cellStyle name="20% - Accent1 2 3 2" xfId="25"/>
+    <cellStyle name="20% - Accent1 2 3 2 2" xfId="28"/>
+    <cellStyle name="20% - Accent1 2 3 2 3" xfId="5"/>
+    <cellStyle name="20% - Accent1 2 3 2 4" xfId="29"/>
+    <cellStyle name="20% - Accent2" xfId="30"/>
+    <cellStyle name="20% - Accent2 2" xfId="32"/>
+    <cellStyle name="20% - Accent2 2 2" xfId="33"/>
+    <cellStyle name="20% - Accent2 2 2 2 2 3" xfId="34"/>
+    <cellStyle name="20% - Accent2 2 2 2 2 3 2" xfId="36"/>
+    <cellStyle name="20% - Accent2 2 2 2 2 3 3" xfId="37"/>
+    <cellStyle name="20% - Accent2 2 3" xfId="35"/>
+    <cellStyle name="20% - Accent2 2 3 2" xfId="9"/>
+    <cellStyle name="20% - Accent3" xfId="39"/>
+    <cellStyle name="20% - Accent4" xfId="40"/>
+    <cellStyle name="20% - Accent5" xfId="42"/>
+    <cellStyle name="20% - Accent6" xfId="16"/>
+    <cellStyle name="40% - Accent1" xfId="3"/>
+    <cellStyle name="40% - Accent1 2" xfId="43"/>
+    <cellStyle name="40% - Accent1 2 2" xfId="45"/>
+    <cellStyle name="40% - Accent1 2 2 2 2 3 2" xfId="48"/>
+    <cellStyle name="40% - Accent1 2 2 2 2 3 2 2" xfId="51"/>
+    <cellStyle name="40% - Accent1 2 2 2 2 3 2 3" xfId="52"/>
+    <cellStyle name="40% - Accent1 2 3" xfId="54"/>
+    <cellStyle name="40% - Accent1 2 3 2" xfId="55"/>
+    <cellStyle name="40% - Accent2" xfId="12"/>
+    <cellStyle name="40% - Accent2 2" xfId="15"/>
+    <cellStyle name="40% - Accent2 2 2" xfId="38"/>
+    <cellStyle name="40% - Accent2 2 2 2 2 3 2" xfId="60"/>
+    <cellStyle name="40% - Accent2 2 2 2 2 3 2 2" xfId="62"/>
+    <cellStyle name="40% - Accent2 2 2 2 2 3 2 3" xfId="31"/>
+    <cellStyle name="40% - Accent2 2 3" xfId="58"/>
+    <cellStyle name="40% - Accent2 2 3 2" xfId="61"/>
+    <cellStyle name="40% - Accent2 2 3 2 2" xfId="138"/>
+    <cellStyle name="40% - Accent2 2 3 2 2 2" xfId="150"/>
+    <cellStyle name="40% - Accent3" xfId="6"/>
+    <cellStyle name="40% - Accent4" xfId="21"/>
+    <cellStyle name="40% - Accent5" xfId="44"/>
+    <cellStyle name="40% - Accent6" xfId="53"/>
+    <cellStyle name="60% - Accent1" xfId="41"/>
+    <cellStyle name="60% - Accent2" xfId="14"/>
+    <cellStyle name="60% - Accent3" xfId="18"/>
+    <cellStyle name="60% - Accent4" xfId="47"/>
+    <cellStyle name="60% - Accent5" xfId="63"/>
+    <cellStyle name="60% - Accent6" xfId="50"/>
+    <cellStyle name="Accent1" xfId="64"/>
+    <cellStyle name="Accent1 2" xfId="65"/>
+    <cellStyle name="Accent1 2 2" xfId="57"/>
+    <cellStyle name="Accent1 2 2 2 2 3" xfId="24"/>
+    <cellStyle name="Accent1 2 2 2 2 3 2" xfId="27"/>
+    <cellStyle name="Accent1 2 2 2 2 3 3" xfId="4"/>
+    <cellStyle name="Accent1 2 3" xfId="66"/>
+    <cellStyle name="Accent1 2 3 2" xfId="69"/>
+    <cellStyle name="Accent1 2 3 2 2" xfId="135"/>
+    <cellStyle name="Accent2" xfId="70"/>
+    <cellStyle name="Accent2 2" xfId="46"/>
+    <cellStyle name="Accent2 2 2" xfId="49"/>
+    <cellStyle name="Accent2 2 2 2 2 3" xfId="71"/>
+    <cellStyle name="Accent2 2 2 2 2 3 2" xfId="72"/>
+    <cellStyle name="Accent2 2 2 2 2 3 3" xfId="73"/>
+    <cellStyle name="Accent2 2 3" xfId="74"/>
+    <cellStyle name="Accent2 2 3 2" xfId="75"/>
+    <cellStyle name="Accent2 2 3 2 2" xfId="136"/>
+    <cellStyle name="Accent3" xfId="76"/>
+    <cellStyle name="Accent4" xfId="23"/>
+    <cellStyle name="Accent5" xfId="77"/>
+    <cellStyle name="Accent6" xfId="26"/>
+    <cellStyle name="Bad" xfId="78"/>
+    <cellStyle name="Calculation" xfId="8"/>
+    <cellStyle name="Check Cell" xfId="79"/>
+    <cellStyle name="Comma [0] 2" xfId="155"/>
+    <cellStyle name="Comma [0] 3" xfId="156"/>
+    <cellStyle name="Explanatory Text" xfId="80"/>
+    <cellStyle name="Good" xfId="81"/>
+    <cellStyle name="Heading 1" xfId="82"/>
+    <cellStyle name="Heading 2" xfId="84"/>
+    <cellStyle name="Heading 2 2" xfId="85"/>
+    <cellStyle name="Heading 2 2 2" xfId="86"/>
+    <cellStyle name="Heading 2 2 2 2 2 3 2" xfId="87"/>
+    <cellStyle name="Heading 2 2 2 2 2 3 2 2" xfId="88"/>
+    <cellStyle name="Heading 2 2 2 2 2 3 2 3" xfId="89"/>
+    <cellStyle name="Heading 2 2 3" xfId="10"/>
+    <cellStyle name="Heading 2 2 3 2" xfId="1"/>
+    <cellStyle name="Heading 3" xfId="90"/>
+    <cellStyle name="Heading 4" xfId="91"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="95" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Hyperlink 4" xfId="96" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Hyperlink 5" xfId="137" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Input" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Linked Cell" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Neutral" xfId="59" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="93"/>
+    <cellStyle name="Hyperlink 2 2" xfId="94"/>
+    <cellStyle name="Hyperlink 3" xfId="95"/>
+    <cellStyle name="Hyperlink 4" xfId="96"/>
+    <cellStyle name="Hyperlink 5" xfId="137"/>
+    <cellStyle name="Input" xfId="97"/>
+    <cellStyle name="Linked Cell" xfId="98"/>
+    <cellStyle name="Neutral" xfId="59"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 2 2 2 2 3 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 2 2 2 2 3 2 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 2 2 2 2 3 2 3" xfId="104" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 2 3" xfId="105" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 2 4" xfId="106" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 2 4 2" xfId="134" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 2 4 2 2" xfId="149" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 2 5" xfId="154" xr:uid="{E10C1125-FCA3-4B99-A82C-864A8C61FBD4}"/>
-    <cellStyle name="Normal 3" xfId="107" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 3 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="109" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="110" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 3 2 4" xfId="140" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Normal 3 2 4 2" xfId="143" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Normal 3 2 4 3" xfId="146" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Normal 3 2 4 3 2" xfId="152" xr:uid="{ED528883-8F94-4628-AF85-5334F7864E90}"/>
-    <cellStyle name="Normal 3 3" xfId="56" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="112" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Normal 3 4" xfId="139" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="151" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Normal 4" xfId="113" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Normal 5" xfId="114" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Note" xfId="68" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Output" xfId="19" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="TableStyleLight1" xfId="115" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="TableStyleLight1 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="TableStyleLight1 2 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="TableStyleLight1 2 2 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="TableStyleLight1 2 2 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="TableStyleLight1 2 2 2 4" xfId="120" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="TableStyleLight1 2 3" xfId="121" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="TableStyleLight1 2 4" xfId="142" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="TableStyleLight1 2 4 2" xfId="145" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="TableStyleLight1 2 4 3" xfId="148" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="TableStyleLight1 3" xfId="122" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="TableStyleLight1 3 2" xfId="123" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="TableStyleLight1 3 2 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="TableStyleLight1 3 2 3" xfId="125" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="TableStyleLight1 3 3" xfId="126" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="TableStyleLight1 3 4" xfId="141" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="TableStyleLight1 3 4 2" xfId="144" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="TableStyleLight1 3 4 3" xfId="147" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="TableStyleLight1 3 4 3 2" xfId="153" xr:uid="{F5250FFE-74D3-4D9A-B0C1-CF3E222169FA}"/>
-    <cellStyle name="TableStyleLight1 4" xfId="67" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="TableStyleLight1 4 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="TableStyleLight1 4 3" xfId="128" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="TableStyleLight1 5" xfId="129" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="TableStyleLight1 5 2" xfId="130" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Title" xfId="131" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Total" xfId="132" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Warning Text" xfId="133" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 2" xfId="99"/>
+    <cellStyle name="Normal 2 2" xfId="100"/>
+    <cellStyle name="Normal 2 2 2" xfId="101"/>
+    <cellStyle name="Normal 2 2 2 2 3 2" xfId="102"/>
+    <cellStyle name="Normal 2 2 2 2 3 2 2" xfId="103"/>
+    <cellStyle name="Normal 2 2 2 2 3 2 3" xfId="104"/>
+    <cellStyle name="Normal 2 3" xfId="105"/>
+    <cellStyle name="Normal 2 4" xfId="106"/>
+    <cellStyle name="Normal 2 4 2" xfId="134"/>
+    <cellStyle name="Normal 2 4 2 2" xfId="149"/>
+    <cellStyle name="Normal 2 5" xfId="154"/>
+    <cellStyle name="Normal 3" xfId="107"/>
+    <cellStyle name="Normal 3 2" xfId="108"/>
+    <cellStyle name="Normal 3 2 2" xfId="109"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="83"/>
+    <cellStyle name="Normal 3 2 3" xfId="110"/>
+    <cellStyle name="Normal 3 2 4" xfId="140"/>
+    <cellStyle name="Normal 3 2 4 2" xfId="143"/>
+    <cellStyle name="Normal 3 2 4 3" xfId="146"/>
+    <cellStyle name="Normal 3 2 4 3 2" xfId="152"/>
+    <cellStyle name="Normal 3 3" xfId="56"/>
+    <cellStyle name="Normal 3 3 2" xfId="111"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="112"/>
+    <cellStyle name="Normal 3 4" xfId="139"/>
+    <cellStyle name="Normal 3 4 2" xfId="151"/>
+    <cellStyle name="Normal 4" xfId="113"/>
+    <cellStyle name="Normal 5" xfId="114"/>
+    <cellStyle name="Note" xfId="68"/>
+    <cellStyle name="Output" xfId="19"/>
+    <cellStyle name="TableStyleLight1" xfId="115"/>
+    <cellStyle name="TableStyleLight1 2" xfId="116"/>
+    <cellStyle name="TableStyleLight1 2 2" xfId="117"/>
+    <cellStyle name="TableStyleLight1 2 2 2" xfId="118"/>
+    <cellStyle name="TableStyleLight1 2 2 2 2" xfId="119"/>
+    <cellStyle name="TableStyleLight1 2 2 2 4" xfId="120"/>
+    <cellStyle name="TableStyleLight1 2 3" xfId="121"/>
+    <cellStyle name="TableStyleLight1 2 4" xfId="142"/>
+    <cellStyle name="TableStyleLight1 2 4 2" xfId="145"/>
+    <cellStyle name="TableStyleLight1 2 4 3" xfId="148"/>
+    <cellStyle name="TableStyleLight1 3" xfId="122"/>
+    <cellStyle name="TableStyleLight1 3 2" xfId="123"/>
+    <cellStyle name="TableStyleLight1 3 2 2" xfId="124"/>
+    <cellStyle name="TableStyleLight1 3 2 3" xfId="125"/>
+    <cellStyle name="TableStyleLight1 3 3" xfId="126"/>
+    <cellStyle name="TableStyleLight1 3 4" xfId="141"/>
+    <cellStyle name="TableStyleLight1 3 4 2" xfId="144"/>
+    <cellStyle name="TableStyleLight1 3 4 3" xfId="147"/>
+    <cellStyle name="TableStyleLight1 3 4 3 2" xfId="153"/>
+    <cellStyle name="TableStyleLight1 4" xfId="67"/>
+    <cellStyle name="TableStyleLight1 4 2" xfId="127"/>
+    <cellStyle name="TableStyleLight1 4 3" xfId="128"/>
+    <cellStyle name="TableStyleLight1 5" xfId="129"/>
+    <cellStyle name="TableStyleLight1 5 2" xfId="130"/>
+    <cellStyle name="Title" xfId="131"/>
+    <cellStyle name="Total" xfId="132"/>
+    <cellStyle name="Warning Text" xfId="133"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2606,18 +2600,10 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="148"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="48"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="48"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2640,25 +2626,22 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.3923741222529194E-2"/>
-          <c:y val="0.1418565099457787"/>
+          <c:x val="5.3923741222529187E-2"/>
+          <c:y val="0.14185650994577867"/>
           <c:w val="0.90694002510216154"/>
-          <c:h val="0.75521895211321821"/>
+          <c:h val="0.75521895211321843"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2673,11 +2656,8 @@
               <a:bevelT w="63500" h="25400"/>
             </a:sp3d>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -2694,7 +2674,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
               </c:ext>
@@ -2702,8 +2682,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="E22B00"/>
@@ -2718,7 +2696,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
               </c:ext>
@@ -2726,8 +2704,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
@@ -2742,7 +2718,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
               </c:ext>
@@ -2750,8 +2726,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
@@ -2766,7 +2740,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
               </c:ext>
@@ -2790,14 +2764,8 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2844,34 +2812,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-71B6-4DE3-A7AD-5B86A9C2BF24}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1420334192"/>
-        <c:axId val="1420343440"/>
+        <c:axId val="62352000"/>
+        <c:axId val="62361984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1420334192"/>
+        <c:axId val="62352000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2885,32 +2841,28 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1420343440"/>
+        <c:crossAx val="62361984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1420343440"/>
+        <c:axId val="62361984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1420334192"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="62352000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:effectLst/>
@@ -2924,25 +2876,17 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="145"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="45"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="45"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2965,24 +2909,12 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
       <c:rotY val="32"/>
-      <c:rAngAx val="0"/>
       <c:perspective val="90"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2990,9 +2922,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.8831278392536694E-2"/>
-          <c:y val="0.14624350369603381"/>
-          <c:w val="0.92496729254319687"/>
-          <c:h val="0.69766331701963358"/>
+          <c:y val="0.14624350369603387"/>
+          <c:w val="0.92496729254319732"/>
+          <c:h val="0.69766331701963369"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -3002,7 +2934,6 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -3011,7 +2942,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-700B-4388-A157-532FE5806D3B}"/>
               </c:ext>
@@ -3019,7 +2950,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:explosion val="19"/>
             <c:spPr>
               <a:solidFill>
@@ -3029,7 +2959,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-700B-4388-A157-532FE5806D3B}"/>
               </c:ext>
@@ -3053,17 +2983,6 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-700B-4388-A157-532FE5806D3B}"/>
-                </c:ext>
-              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
@@ -3082,17 +3001,6 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-700B-4388-A157-532FE5806D3B}"/>
-                </c:ext>
-              </c:extLst>
             </c:dLbl>
             <c:spPr>
               <a:noFill/>
@@ -3101,14 +3009,9 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -3141,20 +3044,14 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-700B-4388-A157-532FE5806D3B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
       </c:pie3DChart>
       <c:spPr>
@@ -3170,16 +3067,14 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.270891046791853"/>
-          <c:y val="0.88141746683253508"/>
-          <c:w val="0.42791036796598075"/>
+          <c:y val="0.88141746683253486"/>
+          <c:w val="0.42791036796598103"/>
           <c:h val="7.1280252974084315E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln w="0"/>
@@ -3193,7 +3088,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -3201,20 +3096,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -3222,9 +3106,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.27595722641494741"/>
-          <c:y val="7.1365887012686355E-2"/>
-          <c:w val="0.29672375522792593"/>
-          <c:h val="0.85466509216403797"/>
+          <c:y val="7.1365887012686383E-2"/>
+          <c:w val="0.29672375522792604"/>
+          <c:h val="0.85466509216403841"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -3239,7 +3123,6 @@
           </c:spPr>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="92D050"/>
@@ -3248,7 +3131,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-D735-4445-9835-790212B0AD76}"/>
               </c:ext>
@@ -3256,7 +3139,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
@@ -3265,7 +3147,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-D735-4445-9835-790212B0AD76}"/>
               </c:ext>
@@ -3273,7 +3155,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
@@ -3282,7 +3163,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-D735-4445-9835-790212B0AD76}"/>
               </c:ext>
@@ -3290,7 +3171,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
@@ -3299,7 +3179,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-D735-4445-9835-790212B0AD76}"/>
               </c:ext>
@@ -3332,10 +3212,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3346,21 +3226,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-D735-4445-9835-790212B0AD76}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -3441,13 +3312,12 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72165251246917395"/>
-          <c:y val="3.608395161789857E-3"/>
+          <c:x val="0.7216525124691745"/>
+          <c:y val="3.6083951617898588E-3"/>
           <c:w val="0.24112408909611374"/>
-          <c:h val="0.95693837006674265"/>
+          <c:h val="0.95693837006674254"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -3474,7 +3344,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3506,7 +3375,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3532,7 +3401,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3570,7 +3439,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3608,7 +3477,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB276036-E4AE-4D63-9C65-0694CB3986A9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB276036-E4AE-4D63-9C65-0694CB3986A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3617,10 +3486,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3640,7 +3509,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3712,7 +3581,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE0DF016-DE8A-4FAD-8AA2-AF2013A5012E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE0DF016-DE8A-4FAD-8AA2-AF2013A5012E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3846,7 +3715,7 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3896,7 +3765,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B7E2C9B-5EB2-4D62-B1DF-88939D760843}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B7E2C9B-5EB2-4D62-B1DF-88939D760843}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4247,7 +4116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4265,33 +4134,33 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:7" ht="18" customHeight="1">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="84" t="s">
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="82" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A7" s="80"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="22" t="s">
         <v>4</v>
       </c>
@@ -4307,7 +4176,7 @@
       <c r="F7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="84"/>
+      <c r="G7" s="82"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickTop="1">
       <c r="A8" s="1" t="s">
@@ -4396,7 +4265,7 @@
     <mergeCell ref="G6:G7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A8" location="'SMART-Multi Product'!A1" display="SMART-Multi Product" xr:uid="{3C04F7C3-0903-46F9-957B-F0A8B92B010E}"/>
+    <hyperlink ref="A8" location="'SMART-Multi Product'!A1" display="SMART-Multi Product"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4405,207 +4274,211 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D286291-DDC2-4806-93E0-E2F89FB5C693}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
     <col min="3" max="3" width="106.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="68" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="141" customHeight="1">
-      <c r="A2" s="85" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="72" t="s">
+      <c r="A2" s="83" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="73" t="s">
-        <v>147</v>
+      <c r="D2" s="70" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="86"/>
-      <c r="B3" s="72" t="s">
+      <c r="A3" s="84"/>
+      <c r="B3" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="74"/>
+      <c r="D3" s="71"/>
     </row>
     <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="86"/>
-      <c r="B4" s="72" t="s">
+      <c r="A4" s="84"/>
+      <c r="B4" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="74"/>
+      <c r="D4" s="71"/>
     </row>
     <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="86"/>
-      <c r="B5" s="72" t="s">
+      <c r="A5" s="84"/>
+      <c r="B5" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="74"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" spans="1:4" ht="15.75">
-      <c r="A6" s="86"/>
-      <c r="B6" s="72" t="s">
+      <c r="A6" s="84"/>
+      <c r="B6" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="71"/>
+    </row>
+    <row r="7" spans="1:4" ht="31.5">
+      <c r="A7" s="84"/>
+      <c r="B7" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="71"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75">
+      <c r="A8" s="84"/>
+      <c r="B8" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="71"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75">
+      <c r="A9" s="84"/>
+      <c r="B9" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="71"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75">
+      <c r="A10" s="84"/>
+      <c r="B10" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75">
+      <c r="A11" s="84"/>
+      <c r="B11" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="71"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75">
+      <c r="A12" s="84"/>
+      <c r="B12" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="71"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75">
+      <c r="A13" s="84"/>
+      <c r="B13" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="71"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75">
+      <c r="A14" s="84"/>
+      <c r="B14" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="71"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75">
+      <c r="A15" s="84"/>
+      <c r="B15" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="71"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75">
+      <c r="A16" s="84"/>
+      <c r="B16" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="71"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75">
+      <c r="A17" s="84"/>
+      <c r="B17" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="71" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75">
+      <c r="A18" s="84"/>
+      <c r="B18" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="74"/>
-    </row>
-    <row r="7" spans="1:4" ht="31.5">
-      <c r="A7" s="86"/>
-      <c r="B7" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="D7" s="74"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75">
-      <c r="A8" s="86"/>
-      <c r="B8" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="74"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75">
-      <c r="A9" s="86"/>
-      <c r="B9" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="74"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75">
-      <c r="A10" s="86"/>
-      <c r="B10" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="74"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75">
-      <c r="A11" s="86"/>
-      <c r="B11" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="74"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75">
-      <c r="A12" s="86"/>
-      <c r="B12" s="72" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="74"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75">
-      <c r="A13" s="86"/>
-      <c r="B13" s="72" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="74"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75">
-      <c r="A14" s="86"/>
-      <c r="B14" s="72" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="74"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75">
-      <c r="A15" s="86"/>
-      <c r="B15" s="72" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="72" t="s">
-        <v>141</v>
-      </c>
-      <c r="D15" s="74"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75">
-      <c r="A16" s="86"/>
-      <c r="B16" s="72" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="74"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75">
-      <c r="A17" s="86"/>
-      <c r="B17" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="74"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75">
-      <c r="A18" s="86"/>
-      <c r="B18" s="72" t="s">
-        <v>154</v>
-      </c>
-      <c r="C18" s="72" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18" s="74"/>
+      <c r="C18" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="71" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="15">
       <c r="C19" s="59"/>
@@ -4646,11 +4519,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65BE7D5C-CCA9-4047-9FB9-7DE5D46B642D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H615"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F153" sqref="F153"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -5316,10 +5189,10 @@
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="35"/>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="97"/>
+      <c r="G2" s="95"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="35"/>
@@ -5378,10 +5251,10 @@
       <c r="C6" s="20"/>
       <c r="D6" s="37"/>
       <c r="E6" s="35"/>
-      <c r="F6" s="98" t="s">
+      <c r="F6" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="99"/>
+      <c r="G6" s="97"/>
     </row>
     <row r="7" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A7" s="35"/>
@@ -5389,7 +5262,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="21">
-        <v>43831</v>
+        <v>43999</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="35"/>
@@ -5398,7 +5271,7 @@
       </c>
       <c r="G7" s="8">
         <f>COUNTIF(G11:G741,"Pass")</f>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1">
@@ -5414,7 +5287,7 @@
       </c>
       <c r="G8" s="8">
         <f>COUNTIF(G12:G742,"Fail")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1">
@@ -5458,7 +5331,7 @@
       </c>
       <c r="C11" s="20">
         <f>G7</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="35"/>
@@ -5472,7 +5345,7 @@
       </c>
       <c r="C12" s="20">
         <f>G8</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="35"/>
@@ -5512,39 +5385,39 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:8" s="40" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="100"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="100"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
       <c r="H16" s="63"/>
     </row>
     <row r="17" spans="1:8" s="40" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="101"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
+      <c r="G17" s="99"/>
       <c r="H17" s="64"/>
     </row>
     <row r="18" spans="1:8" s="40" customFormat="1">
       <c r="A18" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="94"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="95"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="87"/>
       <c r="F18" s="42" t="s">
         <v>28</v>
       </c>
@@ -5558,14 +5431,14 @@
       <c r="A19" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="90" t="s">
+      <c r="B19" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="92"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="90"/>
     </row>
     <row r="20" spans="1:8" s="40" customFormat="1">
       <c r="A20" s="45" t="s">
@@ -5647,27 +5520,27 @@
       <c r="A24" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="89"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="93"/>
     </row>
     <row r="25" spans="1:8" s="40" customFormat="1">
       <c r="A25" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="93" t="s">
+      <c r="B25" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="94" t="s">
+      <c r="C25" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="94" t="s">
+      <c r="D25" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="95" t="s">
+      <c r="E25" s="87" t="s">
         <v>71</v>
       </c>
       <c r="F25" s="42" t="s">
@@ -5682,14 +5555,14 @@
       <c r="A26" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="92"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
     </row>
     <row r="27" spans="1:8" s="40" customFormat="1">
       <c r="A27" s="45" t="s">
@@ -5773,27 +5646,27 @@
       <c r="A31" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="87"/>
-      <c r="C31" s="88"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="89"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="93"/>
     </row>
     <row r="32" spans="1:8" s="40" customFormat="1">
       <c r="A32" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="93" t="s">
+      <c r="B32" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="94" t="s">
+      <c r="C32" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="94" t="s">
+      <c r="D32" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="95" t="s">
+      <c r="E32" s="87" t="s">
         <v>72</v>
       </c>
       <c r="F32" s="42" t="s">
@@ -5808,14 +5681,14 @@
       <c r="A33" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="90" t="s">
+      <c r="B33" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="92"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="90"/>
     </row>
     <row r="34" spans="1:7" s="40" customFormat="1">
       <c r="A34" s="45" t="s">
@@ -5877,14 +5750,14 @@
       <c r="G36" s="50"/>
     </row>
     <row r="37" spans="1:7" s="40" customFormat="1" ht="45">
-      <c r="A37" s="66">
+      <c r="A37" s="46">
         <v>3</v>
       </c>
-      <c r="B37" s="67" t="s">
+      <c r="B37" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="48" t="s">
         <v>149</v>
-      </c>
-      <c r="C37" s="68" t="s">
-        <v>150</v>
       </c>
       <c r="D37" s="48"/>
       <c r="E37" s="48"/>
@@ -5914,27 +5787,27 @@
       <c r="A39" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="87"/>
-      <c r="C39" s="88"/>
-      <c r="D39" s="88"/>
-      <c r="E39" s="88"/>
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="93"/>
     </row>
     <row r="40" spans="1:7" s="40" customFormat="1">
       <c r="A40" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="93" t="s">
+      <c r="B40" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="94" t="s">
+      <c r="C40" s="86" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="94" t="s">
+      <c r="D40" s="86" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="95" t="s">
+      <c r="E40" s="87" t="s">
         <v>76</v>
       </c>
       <c r="F40" s="42" t="s">
@@ -5949,14 +5822,14 @@
       <c r="A41" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="90" t="s">
+      <c r="B41" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="91"/>
-      <c r="D41" s="91"/>
-      <c r="E41" s="91"/>
-      <c r="F41" s="91"/>
-      <c r="G41" s="92"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="90"/>
     </row>
     <row r="42" spans="1:7" s="40" customFormat="1">
       <c r="A42" s="45" t="s">
@@ -6021,11 +5894,11 @@
       <c r="A45" s="66">
         <v>3</v>
       </c>
-      <c r="B45" s="67" t="s">
+      <c r="B45" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" s="48" t="s">
         <v>149</v>
-      </c>
-      <c r="C45" s="68" t="s">
-        <v>150</v>
       </c>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
@@ -6041,8 +5914,8 @@
       <c r="B46" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C46" s="69" t="s">
-        <v>151</v>
+      <c r="C46" s="74" t="s">
+        <v>150</v>
       </c>
       <c r="D46" s="48"/>
       <c r="E46" s="48"/>
@@ -6055,27 +5928,27 @@
       <c r="A47" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="87"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="88"/>
-      <c r="E47" s="88"/>
-      <c r="F47" s="88"/>
-      <c r="G47" s="89"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
+      <c r="E47" s="92"/>
+      <c r="F47" s="92"/>
+      <c r="G47" s="93"/>
     </row>
     <row r="48" spans="1:7" s="40" customFormat="1">
       <c r="A48" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="93" t="s">
-        <v>153</v>
-      </c>
-      <c r="C48" s="94" t="s">
+      <c r="B48" s="85" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="D48" s="94" t="s">
+      <c r="D48" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="E48" s="95" t="s">
+      <c r="E48" s="87" t="s">
         <v>73</v>
       </c>
       <c r="F48" s="42" t="s">
@@ -6197,10 +6070,10 @@
         <v>5</v>
       </c>
       <c r="B55" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D55" s="48"/>
       <c r="E55" s="48"/>
@@ -6214,10 +6087,10 @@
         <v>6</v>
       </c>
       <c r="B56" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D56" s="48"/>
       <c r="E56" s="48"/>
@@ -6228,27 +6101,27 @@
       <c r="A57" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="87"/>
-      <c r="C57" s="88"/>
-      <c r="D57" s="88"/>
-      <c r="E57" s="88"/>
-      <c r="F57" s="88"/>
-      <c r="G57" s="89"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="92"/>
+      <c r="E57" s="92"/>
+      <c r="F57" s="92"/>
+      <c r="G57" s="93"/>
     </row>
     <row r="58" spans="1:7" s="40" customFormat="1">
       <c r="A58" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="93" t="s">
-        <v>155</v>
-      </c>
-      <c r="C58" s="94" t="s">
+      <c r="B58" s="85" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="D58" s="94" t="s">
+      <c r="D58" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="E58" s="95" t="s">
+      <c r="E58" s="87" t="s">
         <v>74</v>
       </c>
       <c r="F58" s="42" t="s">
@@ -6264,7 +6137,7 @@
         <v>29</v>
       </c>
       <c r="B59" s="60" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C59" s="61"/>
       <c r="D59" s="61"/>
@@ -6300,10 +6173,10 @@
         <v>1</v>
       </c>
       <c r="B61" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="48" t="s">
         <v>161</v>
-      </c>
-      <c r="C61" s="48" t="s">
-        <v>162</v>
       </c>
       <c r="D61" s="48"/>
       <c r="E61" s="48"/>
@@ -6315,10 +6188,10 @@
         <v>2</v>
       </c>
       <c r="B62" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" s="48" t="s">
         <v>163</v>
-      </c>
-      <c r="C62" s="48" t="s">
-        <v>164</v>
       </c>
       <c r="D62" s="48"/>
       <c r="E62" s="48"/>
@@ -6329,27 +6202,27 @@
       <c r="A63" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="87"/>
-      <c r="C63" s="88"/>
-      <c r="D63" s="88"/>
-      <c r="E63" s="88"/>
-      <c r="F63" s="88"/>
-      <c r="G63" s="89"/>
+      <c r="B63" s="91"/>
+      <c r="C63" s="92"/>
+      <c r="D63" s="92"/>
+      <c r="E63" s="92"/>
+      <c r="F63" s="92"/>
+      <c r="G63" s="93"/>
     </row>
     <row r="64" spans="1:7" s="40" customFormat="1">
       <c r="A64" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="B64" s="93" t="s">
+      <c r="B64" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="94" t="s">
+      <c r="C64" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="94" t="s">
+      <c r="D64" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="E64" s="95" t="s">
+      <c r="E64" s="87" t="s">
         <v>74</v>
       </c>
       <c r="F64" s="42" t="s">
@@ -6413,7 +6286,7 @@
       </c>
       <c r="G67" s="50"/>
       <c r="H67" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="40" customFormat="1" ht="150">
@@ -6426,7 +6299,7 @@
       <c r="C68" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="D68" s="70" t="s">
+      <c r="D68" s="67" t="s">
         <v>106</v>
       </c>
       <c r="E68" s="48"/>
@@ -6456,27 +6329,27 @@
       <c r="A70" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B70" s="87"/>
-      <c r="C70" s="88"/>
-      <c r="D70" s="88"/>
-      <c r="E70" s="88"/>
-      <c r="F70" s="88"/>
-      <c r="G70" s="89"/>
+      <c r="B70" s="91"/>
+      <c r="C70" s="92"/>
+      <c r="D70" s="92"/>
+      <c r="E70" s="92"/>
+      <c r="F70" s="92"/>
+      <c r="G70" s="93"/>
     </row>
     <row r="71" spans="1:8" s="40" customFormat="1">
       <c r="A71" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="B71" s="93" t="s">
+      <c r="B71" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="C71" s="94" t="s">
+      <c r="C71" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="D71" s="94" t="s">
+      <c r="D71" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="95" t="s">
+      <c r="E71" s="87" t="s">
         <v>75</v>
       </c>
       <c r="F71" s="42" t="s">
@@ -6491,14 +6364,14 @@
       <c r="A72" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B72" s="90" t="s">
+      <c r="B72" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C72" s="91"/>
-      <c r="D72" s="91"/>
-      <c r="E72" s="91"/>
-      <c r="F72" s="91"/>
-      <c r="G72" s="92"/>
+      <c r="C72" s="89"/>
+      <c r="D72" s="89"/>
+      <c r="E72" s="89"/>
+      <c r="F72" s="89"/>
+      <c r="G72" s="90"/>
     </row>
     <row r="73" spans="1:8" s="40" customFormat="1">
       <c r="A73" s="45" t="s">
@@ -6580,27 +6453,27 @@
       <c r="A77" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B77" s="87"/>
-      <c r="C77" s="88"/>
-      <c r="D77" s="88"/>
-      <c r="E77" s="88"/>
-      <c r="F77" s="88"/>
-      <c r="G77" s="89"/>
+      <c r="B77" s="91"/>
+      <c r="C77" s="92"/>
+      <c r="D77" s="92"/>
+      <c r="E77" s="92"/>
+      <c r="F77" s="92"/>
+      <c r="G77" s="93"/>
     </row>
     <row r="78" spans="1:8" s="40" customFormat="1">
       <c r="A78" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="B78" s="93" t="s">
+      <c r="B78" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="C78" s="94" t="s">
+      <c r="C78" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="D78" s="94" t="s">
+      <c r="D78" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="E78" s="95" t="s">
+      <c r="E78" s="87" t="s">
         <v>64</v>
       </c>
       <c r="F78" s="42" t="s">
@@ -6615,14 +6488,14 @@
       <c r="A79" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="90" t="s">
+      <c r="B79" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C79" s="91"/>
-      <c r="D79" s="91"/>
-      <c r="E79" s="91"/>
-      <c r="F79" s="91"/>
-      <c r="G79" s="92"/>
+      <c r="C79" s="89"/>
+      <c r="D79" s="89"/>
+      <c r="E79" s="89"/>
+      <c r="F79" s="89"/>
+      <c r="G79" s="90"/>
     </row>
     <row r="80" spans="1:8" s="40" customFormat="1">
       <c r="A80" s="45" t="s">
@@ -6755,27 +6628,27 @@
       <c r="A87" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B87" s="87"/>
-      <c r="C87" s="88"/>
-      <c r="D87" s="88"/>
-      <c r="E87" s="88"/>
-      <c r="F87" s="88"/>
-      <c r="G87" s="89"/>
+      <c r="B87" s="91"/>
+      <c r="C87" s="92"/>
+      <c r="D87" s="92"/>
+      <c r="E87" s="92"/>
+      <c r="F87" s="92"/>
+      <c r="G87" s="93"/>
     </row>
     <row r="88" spans="1:7" s="40" customFormat="1">
       <c r="A88" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="93" t="s">
+      <c r="B88" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="C88" s="94" t="s">
+      <c r="C88" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="D88" s="94" t="s">
+      <c r="D88" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="E88" s="95" t="s">
+      <c r="E88" s="87" t="s">
         <v>65</v>
       </c>
       <c r="F88" s="42" t="s">
@@ -6790,14 +6663,14 @@
       <c r="A89" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B89" s="90" t="s">
+      <c r="B89" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C89" s="91"/>
-      <c r="D89" s="91"/>
-      <c r="E89" s="91"/>
-      <c r="F89" s="91"/>
-      <c r="G89" s="92"/>
+      <c r="C89" s="89"/>
+      <c r="D89" s="89"/>
+      <c r="E89" s="89"/>
+      <c r="F89" s="89"/>
+      <c r="G89" s="90"/>
     </row>
     <row r="90" spans="1:7" s="40" customFormat="1">
       <c r="A90" s="45" t="s">
@@ -6947,27 +6820,27 @@
       <c r="A98" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B98" s="87"/>
-      <c r="C98" s="88"/>
-      <c r="D98" s="88"/>
-      <c r="E98" s="88"/>
-      <c r="F98" s="88"/>
-      <c r="G98" s="89"/>
+      <c r="B98" s="91"/>
+      <c r="C98" s="92"/>
+      <c r="D98" s="92"/>
+      <c r="E98" s="92"/>
+      <c r="F98" s="92"/>
+      <c r="G98" s="93"/>
     </row>
     <row r="99" spans="1:7" s="40" customFormat="1">
       <c r="A99" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="B99" s="93" t="s">
+      <c r="B99" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="C99" s="94" t="s">
+      <c r="C99" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="D99" s="94" t="s">
+      <c r="D99" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="E99" s="95" t="s">
+      <c r="E99" s="87" t="s">
         <v>66</v>
       </c>
       <c r="F99" s="42" t="s">
@@ -6982,14 +6855,14 @@
       <c r="A100" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B100" s="90" t="s">
+      <c r="B100" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C100" s="91"/>
-      <c r="D100" s="91"/>
-      <c r="E100" s="91"/>
-      <c r="F100" s="91"/>
-      <c r="G100" s="92"/>
+      <c r="C100" s="89"/>
+      <c r="D100" s="89"/>
+      <c r="E100" s="89"/>
+      <c r="F100" s="89"/>
+      <c r="G100" s="90"/>
     </row>
     <row r="101" spans="1:7" s="40" customFormat="1">
       <c r="A101" s="45" t="s">
@@ -7139,27 +7012,27 @@
       <c r="A109" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B109" s="87"/>
-      <c r="C109" s="88"/>
-      <c r="D109" s="88"/>
-      <c r="E109" s="88"/>
-      <c r="F109" s="88"/>
-      <c r="G109" s="89"/>
+      <c r="B109" s="91"/>
+      <c r="C109" s="92"/>
+      <c r="D109" s="92"/>
+      <c r="E109" s="92"/>
+      <c r="F109" s="92"/>
+      <c r="G109" s="93"/>
     </row>
     <row r="110" spans="1:7" s="40" customFormat="1">
       <c r="A110" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B110" s="93" t="s">
+      <c r="B110" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="C110" s="94" t="s">
+      <c r="C110" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="D110" s="94" t="s">
+      <c r="D110" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="E110" s="95" t="s">
+      <c r="E110" s="87" t="s">
         <v>60</v>
       </c>
       <c r="F110" s="42" t="s">
@@ -7174,14 +7047,14 @@
       <c r="A111" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B111" s="90" t="s">
+      <c r="B111" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C111" s="91"/>
-      <c r="D111" s="91"/>
-      <c r="E111" s="91"/>
-      <c r="F111" s="91"/>
-      <c r="G111" s="92"/>
+      <c r="C111" s="89"/>
+      <c r="D111" s="89"/>
+      <c r="E111" s="89"/>
+      <c r="F111" s="89"/>
+      <c r="G111" s="90"/>
     </row>
     <row r="112" spans="1:7" s="40" customFormat="1">
       <c r="A112" s="45" t="s">
@@ -7247,7 +7120,7 @@
       <c r="B115" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="C115" s="76" t="s">
+      <c r="C115" s="73" t="s">
         <v>134</v>
       </c>
       <c r="D115" s="48"/>
@@ -7261,27 +7134,27 @@
       <c r="A116" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B116" s="87"/>
-      <c r="C116" s="88"/>
-      <c r="D116" s="88"/>
-      <c r="E116" s="88"/>
-      <c r="F116" s="88"/>
-      <c r="G116" s="89"/>
+      <c r="B116" s="91"/>
+      <c r="C116" s="92"/>
+      <c r="D116" s="92"/>
+      <c r="E116" s="92"/>
+      <c r="F116" s="92"/>
+      <c r="G116" s="93"/>
     </row>
     <row r="117" spans="1:7" s="40" customFormat="1">
       <c r="A117" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="B117" s="93" t="s">
+      <c r="B117" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="C117" s="94" t="s">
+      <c r="C117" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="D117" s="94" t="s">
+      <c r="D117" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="E117" s="95" t="s">
+      <c r="E117" s="87" t="s">
         <v>135</v>
       </c>
       <c r="F117" s="42" t="s">
@@ -7296,14 +7169,14 @@
       <c r="A118" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B118" s="90" t="s">
+      <c r="B118" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C118" s="91"/>
-      <c r="D118" s="91"/>
-      <c r="E118" s="91"/>
-      <c r="F118" s="91"/>
-      <c r="G118" s="92"/>
+      <c r="C118" s="89"/>
+      <c r="D118" s="89"/>
+      <c r="E118" s="89"/>
+      <c r="F118" s="89"/>
+      <c r="G118" s="90"/>
     </row>
     <row r="119" spans="1:7" s="40" customFormat="1">
       <c r="A119" s="45" t="s">
@@ -7388,7 +7261,7 @@
       <c r="B123" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="C123" s="76" t="s">
+      <c r="C123" s="73" t="s">
         <v>134</v>
       </c>
       <c r="D123" s="48"/>
@@ -7402,27 +7275,27 @@
       <c r="A124" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B124" s="87"/>
-      <c r="C124" s="88"/>
-      <c r="D124" s="88"/>
-      <c r="E124" s="88"/>
-      <c r="F124" s="88"/>
-      <c r="G124" s="89"/>
+      <c r="B124" s="91"/>
+      <c r="C124" s="92"/>
+      <c r="D124" s="92"/>
+      <c r="E124" s="92"/>
+      <c r="F124" s="92"/>
+      <c r="G124" s="93"/>
     </row>
     <row r="125" spans="1:7" s="40" customFormat="1">
       <c r="A125" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B125" s="93" t="s">
+      <c r="B125" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="C125" s="94" t="s">
+      <c r="C125" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="D125" s="94" t="s">
+      <c r="D125" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="E125" s="95" t="s">
+      <c r="E125" s="87" t="s">
         <v>62</v>
       </c>
       <c r="F125" s="42" t="s">
@@ -7437,14 +7310,14 @@
       <c r="A126" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B126" s="90" t="s">
+      <c r="B126" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C126" s="91"/>
-      <c r="D126" s="91"/>
-      <c r="E126" s="91"/>
-      <c r="F126" s="91"/>
-      <c r="G126" s="92"/>
+      <c r="C126" s="89"/>
+      <c r="D126" s="89"/>
+      <c r="E126" s="89"/>
+      <c r="F126" s="89"/>
+      <c r="G126" s="90"/>
     </row>
     <row r="127" spans="1:7" s="40" customFormat="1">
       <c r="A127" s="45" t="s">
@@ -7524,27 +7397,27 @@
       <c r="A131" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B131" s="87"/>
-      <c r="C131" s="88"/>
-      <c r="D131" s="88"/>
-      <c r="E131" s="88"/>
-      <c r="F131" s="88"/>
-      <c r="G131" s="89"/>
+      <c r="B131" s="91"/>
+      <c r="C131" s="92"/>
+      <c r="D131" s="92"/>
+      <c r="E131" s="92"/>
+      <c r="F131" s="92"/>
+      <c r="G131" s="93"/>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B132" s="93" t="s">
+        <v>97</v>
+      </c>
+      <c r="B132" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="C132" s="94" t="s">
+      <c r="C132" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="D132" s="94" t="s">
+      <c r="D132" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="E132" s="95" t="s">
+      <c r="E132" s="87" t="s">
         <v>62</v>
       </c>
       <c r="F132" s="42" t="s">
@@ -7559,14 +7432,14 @@
       <c r="A133" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B133" s="90" t="s">
+      <c r="B133" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C133" s="91"/>
-      <c r="D133" s="91"/>
-      <c r="E133" s="91"/>
-      <c r="F133" s="91"/>
-      <c r="G133" s="92"/>
+      <c r="C133" s="89"/>
+      <c r="D133" s="89"/>
+      <c r="E133" s="89"/>
+      <c r="F133" s="89"/>
+      <c r="G133" s="90"/>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="45" t="s">
@@ -7665,27 +7538,27 @@
       <c r="A139" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B139" s="87"/>
-      <c r="C139" s="88"/>
-      <c r="D139" s="88"/>
-      <c r="E139" s="88"/>
-      <c r="F139" s="88"/>
-      <c r="G139" s="89"/>
+      <c r="B139" s="91"/>
+      <c r="C139" s="92"/>
+      <c r="D139" s="92"/>
+      <c r="E139" s="92"/>
+      <c r="F139" s="92"/>
+      <c r="G139" s="93"/>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B140" s="93" t="s">
+        <v>98</v>
+      </c>
+      <c r="B140" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="C140" s="94" t="s">
+      <c r="C140" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="D140" s="94" t="s">
+      <c r="D140" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="E140" s="95" t="s">
+      <c r="E140" s="87" t="s">
         <v>63</v>
       </c>
       <c r="F140" s="42" t="s">
@@ -7693,21 +7566,21 @@
       </c>
       <c r="G140" s="43" t="str">
         <f>IF(COUNTIF(F143:F145,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F143:F145,"Fail")&gt;0,"Fail",IF(COUNTIF(F143:F145,"")=0,"Pass","Not Executed")))</f>
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="31.5" customHeight="1">
       <c r="A141" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B141" s="90" t="s">
+      <c r="B141" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C141" s="91"/>
-      <c r="D141" s="91"/>
-      <c r="E141" s="91"/>
-      <c r="F141" s="91"/>
-      <c r="G141" s="92"/>
+      <c r="C141" s="89"/>
+      <c r="D141" s="89"/>
+      <c r="E141" s="89"/>
+      <c r="F141" s="89"/>
+      <c r="G141" s="90"/>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="45" t="s">
@@ -7766,7 +7639,7 @@
       </c>
       <c r="G144" s="50"/>
     </row>
-    <row r="145" spans="1:8" ht="75">
+    <row r="145" spans="1:8" ht="45">
       <c r="A145" s="46">
         <v>3</v>
       </c>
@@ -7774,12 +7647,12 @@
         <v>143</v>
       </c>
       <c r="C145" s="48" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="D145" s="48"/>
       <c r="E145" s="48"/>
       <c r="F145" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G145" s="50"/>
     </row>
@@ -7787,49 +7660,49 @@
       <c r="A146" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B146" s="87"/>
-      <c r="C146" s="88"/>
-      <c r="D146" s="88"/>
-      <c r="E146" s="88"/>
-      <c r="F146" s="88"/>
-      <c r="G146" s="89"/>
+      <c r="B146" s="91"/>
+      <c r="C146" s="92"/>
+      <c r="D146" s="92"/>
+      <c r="E146" s="92"/>
+      <c r="F146" s="92"/>
+      <c r="G146" s="93"/>
     </row>
     <row r="147" spans="1:8">
       <c r="A147" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="B147" s="93" t="s">
-        <v>145</v>
-      </c>
-      <c r="C147" s="94" t="s">
+        <v>166</v>
+      </c>
+      <c r="B147" s="85" t="s">
+        <v>144</v>
+      </c>
+      <c r="C147" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="D147" s="94" t="s">
+      <c r="D147" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="E147" s="95" t="s">
+      <c r="E147" s="87" t="s">
         <v>63</v>
       </c>
       <c r="F147" s="42" t="s">
         <v>28</v>
       </c>
       <c r="G147" s="43" t="str">
-        <f>IF(COUNTIF(F150:F152,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F150:F152,"Fail")&gt;0,"Fail",IF(COUNTIF(F150:F152,"")=0,"Pass","Not Executed")))</f>
-        <v>Pass</v>
+        <f>IF(COUNTIF(F150:F153,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F150:F153,"Fail")&gt;0,"Fail",IF(COUNTIF(F150:F153,"")=0,"Pass","Not Executed")))</f>
+        <v>Fail</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="48" customHeight="1">
       <c r="A148" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B148" s="90" t="s">
+      <c r="B148" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C148" s="91"/>
-      <c r="D148" s="91"/>
-      <c r="E148" s="91"/>
-      <c r="F148" s="91"/>
-      <c r="G148" s="92"/>
+      <c r="C148" s="89"/>
+      <c r="D148" s="89"/>
+      <c r="E148" s="89"/>
+      <c r="F148" s="89"/>
+      <c r="G148" s="90"/>
     </row>
     <row r="149" spans="1:8">
       <c r="A149" s="45" t="s">
@@ -7907,20 +7780,20 @@
       </c>
       <c r="G152" s="50"/>
     </row>
-    <row r="153" spans="1:8" ht="75">
+    <row r="153" spans="1:8" ht="45">
       <c r="A153" s="46">
         <v>4</v>
       </c>
       <c r="B153" s="47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C153" s="48" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="D153" s="48"/>
       <c r="E153" s="48"/>
       <c r="F153" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G153" s="50"/>
     </row>
@@ -7928,12 +7801,12 @@
       <c r="A154" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B154" s="87"/>
-      <c r="C154" s="88"/>
-      <c r="D154" s="88"/>
-      <c r="E154" s="88"/>
-      <c r="F154" s="88"/>
-      <c r="G154" s="89"/>
+      <c r="B154" s="91"/>
+      <c r="C154" s="92"/>
+      <c r="D154" s="92"/>
+      <c r="E154" s="92"/>
+      <c r="F154" s="92"/>
+      <c r="G154" s="93"/>
     </row>
     <row r="155" spans="1:8" s="39" customFormat="1" ht="15.75">
       <c r="A155" s="35"/>
@@ -12092,6 +11965,9 @@
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B100:G100"/>
+    <mergeCell ref="B109:G109"/>
+    <mergeCell ref="B110:E110"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B25:E25"/>
@@ -12104,43 +11980,40 @@
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B117:E117"/>
-    <mergeCell ref="B99:E99"/>
-    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B89:G89"/>
+    <mergeCell ref="B98:G98"/>
     <mergeCell ref="B70:G70"/>
     <mergeCell ref="B71:E71"/>
     <mergeCell ref="B72:G72"/>
     <mergeCell ref="B77:G77"/>
     <mergeCell ref="B78:E78"/>
-    <mergeCell ref="B79:G79"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B89:G89"/>
-    <mergeCell ref="B98:G98"/>
-    <mergeCell ref="B100:G100"/>
-    <mergeCell ref="B109:G109"/>
-    <mergeCell ref="B110:E110"/>
-    <mergeCell ref="B111:G111"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="B63:G63"/>
     <mergeCell ref="B148:G148"/>
     <mergeCell ref="B154:G154"/>
+    <mergeCell ref="B146:G146"/>
+    <mergeCell ref="B147:E147"/>
+    <mergeCell ref="B117:E117"/>
     <mergeCell ref="B58:E58"/>
     <mergeCell ref="B133:G133"/>
     <mergeCell ref="B139:G139"/>
     <mergeCell ref="B140:E140"/>
     <mergeCell ref="B141:G141"/>
-    <mergeCell ref="B146:G146"/>
-    <mergeCell ref="B147:E147"/>
     <mergeCell ref="B118:G118"/>
     <mergeCell ref="B124:G124"/>
     <mergeCell ref="B125:E125"/>
     <mergeCell ref="B126:G126"/>
     <mergeCell ref="B131:G131"/>
     <mergeCell ref="B132:E132"/>
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="B64:E64"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F324:F326 F314:F319 F161:F170 F175:F185 F190:F200 F216:F222 F244:F246 F205:F211 F227:F233 F238:F239 F251:F257 F262:F268 F284:F286 F273:F279 F291:F294 F299:F301 F306:F309 F155:F156 F102:F108 F120:F123 F91:F97 F135:F138 F35:F38 F21:F23 F43:F46 F28:F30 F150:F153 F67:F69 F74:F76 F81:F86 F113:F115 F128:F130 F143:F145 F51:F56 F61:F62" xr:uid="{63BD40C3-2F0B-4A04-94AD-178F3E0F2D35}">
+    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F324:F326 F314:F319 F161:F170 F175:F185 F190:F200 F216:F222 F244:F246 F205:F211 F227:F233 F238:F239 F251:F257 F262:F268 F284:F286 F273:F279 F291:F294 F299:F301 F306:F309 F155:F156 F102:F108 F120:F123 F91:F97 F135:F138 F35:F38 F21:F23 F43:F46 F28:F30 F150:F153 F67:F69 F74:F76 F81:F86 F113:F115 F128:F130 F143:F145 F51:F56 F61:F62">
       <formula1>"Pass, Fail, Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>